<commit_message>
Adding dynamics equations to new framework.
</commit_message>
<xml_diff>
--- a/Code/Matlab/Solutions/Main/Precomputed_Network_Simulation/Joint_Data.xlsx
+++ b/Code/Matlab/Solutions/Main/Precomputed_Network_Simulation/Joint_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Code\Matlab\Solutions\Main\Precomputed_Network_Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D57592B-805A-4990-8230-50975DDB1D7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DE5A44-7A6A-4CEA-AEC1-DF79FD18FD51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D94899F0-6C00-4EFE-A0D1-18351498C7BD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Ext</t>
+  </si>
+  <si>
+    <t>Torque</t>
+  </si>
+  <si>
+    <t>[Nm]</t>
   </si>
 </sst>
 </file>
@@ -359,7 +365,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -402,18 +408,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="5" applyBorder="1"/>
@@ -425,6 +419,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
@@ -744,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB170E5-2C31-4C74-A1D7-1C299F2B3E21}">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,87 +779,91 @@
     <col min="16" max="21" width="6.7109375" customWidth="1"/>
     <col min="22" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="39" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39" t="s">
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39" t="s">
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="42" t="s">
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="49" t="s">
         <v>35</v>
       </c>
+      <c r="Z1" s="49" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="40"/>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39" t="s">
+      <c r="K2" s="51"/>
+      <c r="L2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="39"/>
+      <c r="O2" s="51"/>
       <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
@@ -878,9 +891,10 @@
       <c r="X2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="43"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -956,8 +970,11 @@
       <c r="Y3" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="Z3" s="39" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1038,8 +1055,11 @@
       <c r="Y4" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="Z4" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <f>A4+1</f>
         <v>2</v>
@@ -1123,8 +1143,11 @@
       <c r="Y5" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="Z5" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <f t="shared" ref="A6:A17" si="3">A5+1</f>
         <v>3</v>
@@ -1208,8 +1231,11 @@
       <c r="Y6" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="Z6" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1293,8 +1319,11 @@
       <c r="Y7" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="Z7" s="8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1373,11 +1402,14 @@
       <c r="X8" s="14">
         <v>0</v>
       </c>
-      <c r="Y8" s="50" t="s">
+      <c r="Y8" s="46" t="s">
         <v>38</v>
       </c>
+      <c r="Z8" s="46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1458,11 +1490,14 @@
       <c r="X9" s="17">
         <v>0</v>
       </c>
-      <c r="Y9" s="51" t="s">
+      <c r="Y9" s="47" t="s">
         <v>37</v>
       </c>
+      <c r="Z9" s="47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1543,11 +1578,14 @@
       <c r="X10" s="20">
         <v>0</v>
       </c>
-      <c r="Y10" s="52" t="s">
+      <c r="Y10" s="48" t="s">
         <v>38</v>
       </c>
+      <c r="Z10" s="48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1626,11 +1664,14 @@
       <c r="X11" s="23">
         <v>0</v>
       </c>
-      <c r="Y11" s="47" t="s">
+      <c r="Y11" s="43" t="s">
         <v>37</v>
       </c>
+      <c r="Z11" s="43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1711,11 +1752,14 @@
       <c r="X12" s="26">
         <v>0</v>
       </c>
-      <c r="Y12" s="48" t="s">
+      <c r="Y12" s="44" t="s">
         <v>37</v>
       </c>
+      <c r="Z12" s="44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1796,11 +1840,14 @@
       <c r="X13" s="26">
         <v>0</v>
       </c>
-      <c r="Y13" s="48" t="s">
+      <c r="Y13" s="44" t="s">
         <v>38</v>
       </c>
+      <c r="Z13" s="44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1881,11 +1928,14 @@
       <c r="X14" s="29">
         <v>0</v>
       </c>
-      <c r="Y14" s="49" t="s">
+      <c r="Y14" s="45" t="s">
         <v>38</v>
       </c>
+      <c r="Z14" s="45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1964,11 +2014,14 @@
       <c r="X15" s="32">
         <v>0</v>
       </c>
-      <c r="Y15" s="44" t="s">
+      <c r="Y15" s="40" t="s">
         <v>38</v>
       </c>
+      <c r="Z15" s="40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2049,11 +2102,14 @@
       <c r="X16" s="35">
         <v>0</v>
       </c>
-      <c r="Y16" s="45" t="s">
+      <c r="Y16" s="41" t="s">
         <v>37</v>
       </c>
+      <c r="Z16" s="41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -2134,28 +2190,32 @@
       <c r="X17" s="38">
         <v>0</v>
       </c>
-      <c r="Y17" s="46" t="s">
+      <c r="Y17" s="42" t="s">
         <v>38</v>
+      </c>
+      <c r="Z17" s="42">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+  <mergeCells count="17">
+    <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>